<commit_message>
cn-#14 Add FileDiff end of file check
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB32389-F0CC-40FB-B37F-62004EA337E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878BD59C-C98B-47F9-8350-E22B40E16EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
+    <sheet name="SumProduct" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Scenario</t>
   </si>
@@ -66,6 +67,15 @@
   </si>
   <si>
     <t>First Number</t>
+  </si>
+  <si>
+    <t>SumProduct Function</t>
+  </si>
+  <si>
+    <t>I have following two list of numbers</t>
+  </si>
+  <si>
+    <t>call the SumProduct Function</t>
   </si>
 </sst>
 </file>
@@ -385,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,4 +461,90 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56A2648-9341-4E85-9598-42A965E1B406}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>-3</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <f>SUMPRODUCT(B5:B7,C5:C7)</f>
+        <v>3503</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add verify step to test SumProduct function
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878BD59C-C98B-47F9-8350-E22B40E16EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F54BE-3BA3-4A4A-A0F1-21C9CCC0EA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
     <t>I have following two list of numbers</t>
   </si>
   <si>
-    <t>call the SumProduct Function</t>
+    <t>I call the SumProduct function</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cn-#14 add ignoreTableFormat option when comparing files.
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112F54BE-3BA3-4A4A-A0F1-21C9CCC0EA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F65C4-31E7-4733-9CA9-4B07633F471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56A2648-9341-4E85-9598-42A965E1B406}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -500,31 +500,49 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>50</v>
       </c>
       <c r="C5">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f>B5*C5*D5</f>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E7" si="0">B6*C6*D6</f>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>-3</v>
       </c>
-      <c r="C7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -532,7 +550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -540,8 +558,8 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <f>SUMPRODUCT(B5:B7,C5:C7)</f>
-        <v>3503</v>
+        <f>SUMPRODUCT(B5:B7,C5:C7, D5:D7)</f>
+        <v>7576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cn-#14 rollback unintended testing case change
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6F65C4-31E7-4733-9CA9-4B07633F471A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CEC58C-78D1-49EB-A3EC-05101CE5778E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56A2648-9341-4E85-9598-42A965E1B406}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D5" sqref="D5:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -500,49 +500,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>50</v>
       </c>
       <c r="C5">
         <v>70</v>
       </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <f>B5*C5*D5</f>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <f t="shared" ref="E6:E7" si="0">B6*C6*D6</f>
-        <v>576</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>-3</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -550,7 +532,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -558,8 +540,8 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <f>SUMPRODUCT(B5:B7,C5:C7, D5:D7)</f>
-        <v>7576</v>
+        <f>SUMPRODUCT(B5:B7,C5:C7)</f>
+        <v>3515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cn-#18 Add should Ignored cells to data table testing.
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CEC58C-78D1-49EB-A3EC-05101CE5778E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7E2D2C-0D8C-46B4-8A76-198D9A155BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2730" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>Scenario</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>I call the SumProduct function</t>
+  </si>
+  <si>
+    <t>Ignored</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>Ignored after two empty cells</t>
   </si>
 </sst>
 </file>
@@ -465,18 +477,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56A2648-9341-4E85-9598-42A965E1B406}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:E7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -492,39 +505,51 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>50</v>
       </c>
       <c r="C5">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>-3</v>
       </c>
       <c r="C7">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -532,7 +557,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
cn-#18 ignore columns after one empty cell in table header
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7E2D2C-0D8C-46B4-8A76-198D9A155BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A397451-0356-49D3-BD37-285DE8664EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26205" yWindow="4200" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
     <t>be</t>
   </si>
   <si>
-    <t>Ignored after two empty cells</t>
+    <t>Ignored after an empty cells on a table</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56A2648-9341-4E85-9598-42A965E1B406}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cn-#18 make sure table rows will not be ignored due to empty space
</commit_message>
<xml_diff>
--- a/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
+++ b/test/Cactus.ReqnrollConveterTest/Features/DataGridSample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\itu\Cactus.net\test\Cactus.ReqnrollConveterTest\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A397451-0356-49D3-BD37-285DE8664EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306EB938-2E7E-42C7-895E-69113592F9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26205" yWindow="4200" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddTwoNumbers" sheetId="1" r:id="rId1"/>
     <sheet name="SumProduct" sheetId="2" r:id="rId2"/>
+    <sheet name="SumAverage" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Scenario</t>
   </si>
@@ -72,9 +73,6 @@
     <t>SumProduct Function</t>
   </si>
   <si>
-    <t>I have following two list of numbers</t>
-  </si>
-  <si>
     <t>I call the SumProduct function</t>
   </si>
   <si>
@@ -88,6 +86,33 @@
   </si>
   <si>
     <t>Ignored after an empty cells on a table</t>
+  </si>
+  <si>
+    <t>I have following list of numbers</t>
+  </si>
+  <si>
+    <t>Third Number</t>
+  </si>
+  <si>
+    <t>Forth Number</t>
+  </si>
+  <si>
+    <t>#Avg</t>
+  </si>
+  <si>
+    <t>I call the SumAverage function</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>To test that table value will not be ignored due to empty space</t>
+  </si>
+  <si>
+    <t>For simplify testing purpose, I made the roll average full integer.</t>
+  </si>
+  <si>
+    <t>SumAverage Function</t>
   </si>
 </sst>
 </file>
@@ -407,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +505,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -513,7 +538,7 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -524,7 +549,7 @@
         <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -535,7 +560,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -546,7 +571,7 @@
         <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -554,7 +579,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -567,6 +592,151 @@
       <c r="C11">
         <f>SUMPRODUCT(B5:B7,C5:C7)</f>
         <v>3515</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF114F8-AE7E-4D14-A136-FB162BCC3B37}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(B7:E7)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ref="H8:H10" si="0">AVERAGE(B8:E8)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>-3</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <f>SUM(H7:H10)</f>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>